<commit_message>
modificando arquivo output modelo e formatando os dados para padrão numérico
</commit_message>
<xml_diff>
--- a/RPA_Teste/Pipes/Excel/Archives/OutputModel.xlsx
+++ b/RPA_Teste/Pipes/Excel/Archives/OutputModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\Finanças\Rpa_Challenge\RPA_Teste\bin\Debug\net8.0\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707F6C8E-3410-4903-A3DC-E7FB69199988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365EEBD0-0952-4C72-8B2D-E2F548FFF97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acoes" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +123,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,15 +160,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,38 +457,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="2"/>
-    <col min="10" max="10" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -488,13 +496,13 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -514,15 +522,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E0E4E5-844A-4AB4-9F41-6B49128F3BE8}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -537,10 +545,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -555,10 +563,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -567,18 +575,21 @@
       <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>